<commit_message>
Updated comments to case study
</commit_message>
<xml_diff>
--- a/data/results.xlsx
+++ b/data/results.xlsx
@@ -437,19 +437,19 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.1452793956164414</v>
+        <v>0.1452794114198362</v>
       </c>
       <c r="C3">
-        <v>0.1433159803172872</v>
+        <v>0.143315996105127</v>
       </c>
       <c r="D3">
-        <v>0.1403708541705296</v>
+        <v>0.1403708699680404</v>
       </c>
       <c r="E3">
-        <v>0.1433159803172877</v>
+        <v>0.143315996105127</v>
       </c>
       <c r="F3">
-        <v>0.1403708541705296</v>
+        <v>0.1403708699680404</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -457,19 +457,19 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.1816369129819771</v>
+        <v>0.181636899529273</v>
       </c>
       <c r="C4">
-        <v>0.1773456704932926</v>
+        <v>0.1773456570630396</v>
       </c>
       <c r="D4">
-        <v>0.1706027254407327</v>
+        <v>0.1706027120175976</v>
       </c>
       <c r="E4">
-        <v>0.1773456805354048</v>
+        <v>0.1773456671051518</v>
       </c>
       <c r="F4">
-        <v>0.1706027330918664</v>
+        <v>0.1706027196687313</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -477,19 +477,19 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.2371403903786543</v>
+        <v>0.2371404008424781</v>
       </c>
       <c r="C5">
-        <v>0.2278604446043252</v>
+        <v>0.2278604550698377</v>
       </c>
       <c r="D5">
-        <v>0.2129280132196407</v>
+        <v>0.212928023711534</v>
       </c>
       <c r="E5">
-        <v>0.2278605586207613</v>
+        <v>0.2278605690862731</v>
       </c>
       <c r="F5">
-        <v>0.2129281001032337</v>
+        <v>0.2129281105951265</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -497,19 +497,19 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.3260461147306919</v>
+        <v>0.3260461146391306</v>
       </c>
       <c r="C6">
-        <v>0.3062807393049019</v>
+        <v>0.3062807392404065</v>
       </c>
       <c r="D6">
-        <v>0.2740728580018133</v>
+        <v>0.2740728579822234</v>
       </c>
       <c r="E6">
-        <v>0.3062815980351761</v>
+        <v>0.3062815979706786</v>
       </c>
       <c r="F6">
-        <v>0.2740735125482718</v>
+        <v>0.2740735125286804</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -517,19 +517,19 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.4739438218527361</v>
+        <v>0.4739438216727918</v>
       </c>
       <c r="C7">
-        <v>0.4326388686060117</v>
+        <v>0.4326388684787959</v>
       </c>
       <c r="D7">
-        <v>0.3648649212699454</v>
+        <v>0.3648649212302039</v>
       </c>
       <c r="E7">
-        <v>0.4326441601048017</v>
+        <v>0.432644159977573</v>
       </c>
       <c r="F7">
-        <v>0.3648689561718996</v>
+        <v>0.3648689561321471</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -537,19 +537,19 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.7257883745591727</v>
+        <v>0.7257883742173169</v>
       </c>
       <c r="C8">
-        <v>0.6415300899866518</v>
+        <v>0.6415300897436407</v>
       </c>
       <c r="D8">
-        <v>0.502735251599722</v>
+        <v>0.5027352515206882</v>
       </c>
       <c r="E8">
-        <v>0.6415584732346775</v>
+        <v>0.6415584729916034</v>
       </c>
       <c r="F8">
-        <v>0.502756907156237</v>
+        <v>0.5027569070771498</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -557,19 +557,19 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>1.157953982833573</v>
+        <v>1.157953982210619</v>
       </c>
       <c r="C9">
-        <v>0.9913027483552628</v>
+        <v>0.9913027479087756</v>
       </c>
       <c r="D9">
-        <v>0.7161644273522541</v>
+        <v>0.7161644271984507</v>
       </c>
       <c r="E9">
-        <v>0.9914380974348056</v>
+        <v>0.9914380969880195</v>
       </c>
       <c r="F9">
-        <v>0.7162677851241712</v>
+        <v>0.7162677849701446</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -577,19 +577,19 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>1.893714521149819</v>
+        <v>1.8937145200725</v>
       </c>
       <c r="C10">
-        <v>1.576657149776699</v>
+        <v>1.576657148994824</v>
       </c>
       <c r="D10">
-        <v>1.052525798258275</v>
+        <v>1.052525797966322</v>
       </c>
       <c r="E10">
-        <v>1.577234130110696</v>
+        <v>1.577234129327625</v>
       </c>
       <c r="F10">
-        <v>1.052966998482337</v>
+        <v>1.052966998189475</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -597,19 +597,19 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>3.117384905151875</v>
+        <v>3.117384903408206</v>
       </c>
       <c r="C11">
-        <v>2.542224188949457</v>
+        <v>2.542224187659234</v>
       </c>
       <c r="D11">
-        <v>1.590812407744154</v>
+        <v>1.590812407205306</v>
       </c>
       <c r="E11">
-        <v>2.544420621010353</v>
+        <v>2.544420619715842</v>
       </c>
       <c r="F11">
-        <v>1.592495543873835</v>
+        <v>1.592495543331717</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -617,19 +617,19 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>5.075886168001927</v>
+        <v>5.075886165411384</v>
       </c>
       <c r="C12">
-        <v>4.090565074660808</v>
+        <v>4.090565072683283</v>
       </c>
       <c r="D12">
-        <v>2.460583562961397</v>
+        <v>2.460583561998068</v>
       </c>
       <c r="E12">
-        <v>4.098001450553171</v>
+        <v>4.098001448562234</v>
       </c>
       <c r="F12">
-        <v>2.466301647828478</v>
+        <v>2.466301646854812</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -637,19 +637,19 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>8.050410223640499</v>
+        <v>8.050410220214424</v>
       </c>
       <c r="C13">
-        <v>6.473771858271517</v>
+        <v>6.473771855513168</v>
       </c>
       <c r="D13">
-        <v>3.86750015882602</v>
+        <v>3.867500157166094</v>
       </c>
       <c r="E13">
-        <v>6.496036090917871</v>
+        <v>6.496036088122731</v>
       </c>
       <c r="F13">
-        <v>3.884715042678983</v>
+        <v>3.884715040990486</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -657,19 +657,19 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>12.28034780850724</v>
+        <v>12.28034780470608</v>
       </c>
       <c r="C14">
-        <v>9.954843442576143</v>
+        <v>9.954843439185744</v>
       </c>
       <c r="D14">
-        <v>6.119302983291395</v>
+        <v>6.119302980552657</v>
       </c>
       <c r="E14">
-        <v>10.01337234288319</v>
+        <v>10.01337233940569</v>
       </c>
       <c r="F14">
-        <v>6.164966136839291</v>
+        <v>6.164966134032177</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -677,19 +677,19 @@
         <v>2024</v>
       </c>
       <c r="B15">
-        <v>17.84594559111853</v>
+        <v>17.84594558812026</v>
       </c>
       <c r="C15">
-        <v>14.73637621497504</v>
+        <v>14.7363762115254</v>
       </c>
       <c r="D15">
-        <v>9.637085805705093</v>
+        <v>9.637085801418221</v>
       </c>
       <c r="E15">
-        <v>14.8702930975608</v>
+        <v>14.87029309393616</v>
       </c>
       <c r="F15">
-        <v>9.743094320926836</v>
+        <v>9.743094316499588</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -697,19 +697,19 @@
         <v>2025</v>
       </c>
       <c r="B16">
-        <v>24.56353494582056</v>
+        <v>24.56353494556669</v>
       </c>
       <c r="C16">
-        <v>20.87561820892671</v>
+        <v>20.87561820649562</v>
       </c>
       <c r="D16">
-        <v>14.91616273411089</v>
+        <v>14.9161627278273</v>
       </c>
       <c r="E16">
-        <v>21.13935316608367</v>
+        <v>21.13935316336207</v>
       </c>
       <c r="F16">
-        <v>15.12991302445179</v>
+        <v>15.12991301792625</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -717,19 +717,19 @@
         <v>2026</v>
       </c>
       <c r="B17">
-        <v>32.00223673392776</v>
+        <v>32.00223673862452</v>
       </c>
       <c r="C17">
-        <v>28.23652445313708</v>
+        <v>28.23652445310658</v>
       </c>
       <c r="D17">
-        <v>22.39129842383162</v>
+        <v>22.3912984153693</v>
       </c>
       <c r="E17">
-        <v>28.67705295121928</v>
+        <v>28.67705295080986</v>
       </c>
       <c r="F17">
-        <v>22.76240670946885</v>
+        <v>22.76240670066617</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -737,19 +737,19 @@
         <v>2027</v>
       </c>
       <c r="B18">
-        <v>39.7073232823016</v>
+        <v>39.70732329325847</v>
       </c>
       <c r="C18">
-        <v>36.52746078230073</v>
+        <v>36.52746078579545</v>
       </c>
       <c r="D18">
-        <v>32.18510508988952</v>
+        <v>32.18510507972336</v>
       </c>
       <c r="E18">
-        <v>37.13857475722714</v>
+        <v>37.13857476038252</v>
       </c>
       <c r="F18">
-        <v>32.73460693821486</v>
+        <v>32.7346069276806</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -757,19 +757,19 @@
         <v>2028</v>
       </c>
       <c r="B19">
-        <v>47.5392588975297</v>
+        <v>47.53925891380706</v>
       </c>
       <c r="C19">
-        <v>45.40212167057719</v>
+        <v>45.40212167776431</v>
       </c>
       <c r="D19">
-        <v>43.80379677665578</v>
+        <v>43.80379676631915</v>
       </c>
       <c r="E19">
-        <v>46.08190989489035</v>
+        <v>46.08190990199229</v>
       </c>
       <c r="F19">
-        <v>44.49052395477405</v>
+        <v>44.49052394417939</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -777,19 +777,19 @@
         <v>2029</v>
       </c>
       <c r="B20">
-        <v>55.82731637040401</v>
+        <v>55.82731638831743</v>
       </c>
       <c r="C20">
-        <v>54.52359563081477</v>
+        <v>54.52359564056853</v>
       </c>
       <c r="D20">
-        <v>55.9793940270566</v>
+        <v>55.97939401923466</v>
       </c>
       <c r="E20">
-        <v>55.08416664051032</v>
+        <v>55.08416665062494</v>
       </c>
       <c r="F20">
-        <v>56.69552095388492</v>
+        <v>56.69552094605898</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -797,19 +797,19 @@
         <v>2030</v>
       </c>
       <c r="B21">
-        <v>65.11720347360615</v>
+        <v>65.11720348787973</v>
       </c>
       <c r="C21">
-        <v>63.55240739020626</v>
+        <v>63.55240740050182</v>
       </c>
       <c r="D21">
-        <v>66.92123157286724</v>
+        <v>66.9212315708471</v>
       </c>
       <c r="E21">
-        <v>63.80374657117482</v>
+        <v>63.80374658229563</v>
       </c>
       <c r="F21">
-        <v>67.53936109017269</v>
+        <v>67.53936108845268</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -817,19 +817,19 @@
         <v>2031</v>
       </c>
       <c r="B22">
-        <v>75.66094315505545</v>
+        <v>75.66094316116725</v>
       </c>
       <c r="C22">
-        <v>72.12404234082258</v>
+        <v>72.12404234963044</v>
       </c>
       <c r="D22">
-        <v>74.97926924886553</v>
+        <v>74.97926925535722</v>
       </c>
       <c r="E22">
-        <v>71.98747153157917</v>
+        <v>71.98747154147391</v>
       </c>
       <c r="F22">
-        <v>75.42866686934143</v>
+        <v>75.4286668763193</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -837,19 +837,19 @@
         <v>2032</v>
       </c>
       <c r="B23">
-        <v>87.0893963400008</v>
+        <v>87.08939633620051</v>
       </c>
       <c r="C23">
-        <v>79.9081967912868</v>
+        <v>79.90819679731445</v>
       </c>
       <c r="D23">
-        <v>79.34211421368128</v>
+        <v>79.34211422955241</v>
       </c>
       <c r="E23">
-        <v>79.47788988120655</v>
+        <v>79.47788988822282</v>
       </c>
       <c r="F23">
-        <v>79.65470100113204</v>
+        <v>79.65470101743888</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -857,19 +857,19 @@
         <v>2033</v>
       </c>
       <c r="B24">
-        <v>98.52266938619343</v>
+        <v>98.52266937397127</v>
       </c>
       <c r="C24">
-        <v>86.72381997500511</v>
+        <v>86.72381997786054</v>
       </c>
       <c r="D24">
-        <v>80.31619316210551</v>
+        <v>80.31619318576575</v>
       </c>
       <c r="E24">
-        <v>86.22805586558535</v>
+        <v>86.22805586897685</v>
       </c>
       <c r="F24">
-        <v>80.60319301658272</v>
+        <v>80.60319304040273</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -877,19 +877,19 @@
         <v>2034</v>
       </c>
       <c r="B25">
-        <v>108.9469920629921</v>
+        <v>108.9469920460467</v>
       </c>
       <c r="C25">
-        <v>92.58232810426553</v>
+        <v>92.58232810417401</v>
       </c>
       <c r="D25">
-        <v>79.05424991397446</v>
+        <v>79.05424994176178</v>
       </c>
       <c r="E25">
-        <v>92.27343916474855</v>
+        <v>92.27343916456786</v>
       </c>
       <c r="F25">
-        <v>79.43140286116142</v>
+        <v>79.43140288876261</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -897,19 +897,19 @@
         <v>2035</v>
       </c>
       <c r="B26">
-        <v>117.557604191298</v>
+        <v>117.5576041739363</v>
       </c>
       <c r="C26">
-        <v>97.61698202943705</v>
+        <v>97.61698202691524</v>
       </c>
       <c r="D26">
-        <v>76.99425954881596</v>
+        <v>76.99425957614596</v>
       </c>
       <c r="E26">
-        <v>97.66471309996983</v>
+        <v>97.66471309680489</v>
       </c>
       <c r="F26">
-        <v>77.50896223551078</v>
+        <v>77.50896226246357</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -917,19 +917,19 @@
         <v>2036</v>
       </c>
       <c r="B27">
-        <v>123.9162698662939</v>
+        <v>123.9162698521243</v>
       </c>
       <c r="C27">
-        <v>101.9625982358432</v>
+        <v>101.962598231546</v>
       </c>
       <c r="D27">
-        <v>75.35072739044161</v>
+        <v>75.35072741313388</v>
       </c>
       <c r="E27">
-        <v>102.4069987704438</v>
+        <v>102.4069987652174</v>
       </c>
       <c r="F27">
-        <v>75.95372905025532</v>
+        <v>75.95372907267084</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -937,19 +937,19 @@
         <v>2037</v>
       </c>
       <c r="B28">
-        <v>127.9598570982844</v>
+        <v>127.9598570895414</v>
       </c>
       <c r="C28">
-        <v>105.6829128261556</v>
+        <v>105.6829128208506</v>
       </c>
       <c r="D28">
-        <v>74.85591577684941</v>
+        <v>74.8559157920937</v>
       </c>
       <c r="E28">
-        <v>106.4519398625429</v>
+        <v>106.4519398563537</v>
       </c>
       <c r="F28">
-        <v>75.42637692710413</v>
+        <v>75.42637694246068</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -957,19 +957,19 @@
         <v>2038</v>
       </c>
       <c r="B29">
-        <v>129.935885203364</v>
+        <v>129.9358852007719</v>
       </c>
       <c r="C29">
-        <v>108.7731744428371</v>
+        <v>108.773174437368</v>
       </c>
       <c r="D29">
-        <v>75.74771641600975</v>
+        <v>75.74771642272137</v>
       </c>
       <c r="E29">
-        <v>109.7359649250804</v>
+        <v>109.735964919024</v>
       </c>
       <c r="F29">
-        <v>76.15271769838249</v>
+        <v>76.15271770573014</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -977,19 +977,19 @@
         <v>2039</v>
       </c>
       <c r="B30">
-        <v>130.3174645947398</v>
+        <v>130.3174645977118</v>
       </c>
       <c r="C30">
-        <v>111.2131401028428</v>
+        <v>111.2131400980147</v>
       </c>
       <c r="D30">
-        <v>77.90605946531332</v>
+        <v>77.90605946395566</v>
       </c>
       <c r="E30">
-        <v>112.235090291328</v>
+        <v>112.235090286304</v>
       </c>
       <c r="F30">
-        <v>78.06399167568485</v>
+        <v>78.0639916753946</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -997,19 +997,19 @@
         <v>2040</v>
       </c>
       <c r="B31">
-        <v>129.6989653333128</v>
+        <v>129.6989653403162</v>
       </c>
       <c r="C31">
-        <v>113.0119999553634</v>
+        <v>113.0119999517926</v>
       </c>
       <c r="D31">
-        <v>81.01452962648349</v>
+        <v>81.01452961857566</v>
       </c>
       <c r="E31">
-        <v>113.9901366617478</v>
+        <v>113.9901366583156</v>
       </c>
       <c r="F31">
-        <v>80.9339833211085</v>
+        <v>80.93398331440753</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1017,19 +1017,19 @@
         <v>2041</v>
       </c>
       <c r="B32">
-        <v>128.6915392266613</v>
+        <v>128.6915392356644</v>
       </c>
       <c r="C32">
-        <v>114.2317874783402</v>
+        <v>114.2317874763442</v>
       </c>
       <c r="D32">
-        <v>84.69278076723276</v>
+        <v>84.69278075480274</v>
       </c>
       <c r="E32">
-        <v>115.106434513732</v>
+        <v>115.1064345120727</v>
       </c>
       <c r="F32">
-        <v>84.47403216659201</v>
+        <v>84.47403215513611</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1037,19 +1037,19 @@
         <v>2042</v>
       </c>
       <c r="B33">
-        <v>127.8238196671548</v>
+        <v>127.8238196760824</v>
       </c>
       <c r="C33">
-        <v>114.9812891767805</v>
+        <v>114.9812891763529</v>
       </c>
       <c r="D33">
-        <v>88.57367965449309</v>
+        <v>88.57367963964403</v>
       </c>
       <c r="E33">
-        <v>115.7310966829154</v>
+        <v>115.7310966828804</v>
       </c>
       <c r="F33">
-        <v>88.37573131799529</v>
+        <v>88.37573130357379</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1057,19 +1057,19 @@
         <v>2043</v>
       </c>
       <c r="B34">
-        <v>127.4670597958154</v>
+        <v>127.467059802948</v>
       </c>
       <c r="C34">
-        <v>115.3952976439212</v>
+        <v>115.3952976447941</v>
       </c>
       <c r="D34">
-        <v>92.33803381698746</v>
+        <v>92.33803380162421</v>
       </c>
       <c r="E34">
-        <v>116.025955146075</v>
+        <v>116.0259551472961</v>
       </c>
       <c r="F34">
-        <v>92.32732981754157</v>
+        <v>92.3273298019144</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1077,19 +1077,19 @@
         <v>2044</v>
       </c>
       <c r="B35">
-        <v>127.7952886377703</v>
+        <v>127.795288642025</v>
       </c>
       <c r="C35">
-        <v>115.6089862751711</v>
+        <v>115.6089862769247</v>
       </c>
       <c r="D35">
-        <v>95.72287977925964</v>
+        <v>95.72287976496281</v>
       </c>
       <c r="E35">
-        <v>116.142733986178</v>
+        <v>116.142733988184</v>
       </c>
       <c r="F35">
-        <v>96.02447710944574</v>
+        <v>96.02447709424801</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1097,19 +1097,19 @@
         <v>2045</v>
       </c>
       <c r="B36">
-        <v>128.791362678857</v>
+        <v>128.7913626799032</v>
       </c>
       <c r="C36">
-        <v>115.7409848855948</v>
+        <v>115.7409848877676</v>
       </c>
       <c r="D36">
-        <v>98.52490547987009</v>
+        <v>98.5249054678544</v>
       </c>
       <c r="E36">
-        <v>116.2088089849927</v>
+        <v>116.2088089873104</v>
       </c>
       <c r="F36">
-        <v>99.19250744003938</v>
+        <v>99.19250742670073</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1117,19 +1117,19 @@
         <v>2046</v>
       </c>
       <c r="B37">
-        <v>130.2890102103233</v>
+        <v>130.2890102085246</v>
       </c>
       <c r="C37">
-        <v>115.8831134211365</v>
+        <v>115.8831134233124</v>
       </c>
       <c r="D37">
-        <v>100.6030161706117</v>
+        <v>100.6030161617199</v>
       </c>
       <c r="E37">
-        <v>116.3189575242303</v>
+        <v>116.3189575264526</v>
       </c>
       <c r="F37">
-        <v>101.6135807398806</v>
+        <v>101.6135807295337</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1137,19 +1137,19 @@
         <v>2047</v>
       </c>
       <c r="B38">
-        <v>132.0370451218019</v>
+        <v>132.0370451180287</v>
       </c>
       <c r="C38">
-        <v>116.0960127497137</v>
+        <v>116.0960127515764</v>
       </c>
       <c r="D38">
-        <v>101.8821145823982</v>
+        <v>101.8821145771072</v>
       </c>
       <c r="E38">
-        <v>116.5319653509278</v>
+        <v>116.5319653527551</v>
       </c>
       <c r="F38">
-        <v>103.1513468621392</v>
+        <v>103.151346855543</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1157,19 +1157,19 @@
         <v>2048</v>
       </c>
       <c r="B39">
-        <v>133.7692167127189</v>
+        <v>133.7692167080786</v>
       </c>
       <c r="C39">
-        <v>116.4098699905043</v>
+        <v>116.4098699918542</v>
       </c>
       <c r="D39">
-        <v>102.3572318101162</v>
+        <v>102.3572318085403</v>
       </c>
       <c r="E39">
-        <v>116.8720105134236</v>
+        <v>116.8720105146785</v>
       </c>
       <c r="F39">
-        <v>103.7665679136505</v>
+        <v>103.7665679111272</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1177,19 +1177,19 @@
         <v>2049</v>
       </c>
       <c r="B40">
-        <v>135.2657387848821</v>
+        <v>135.2657387804554</v>
       </c>
       <c r="C40">
-        <v>116.830657866811</v>
+        <v>116.8306578675684</v>
       </c>
       <c r="D40">
-        <v>102.0966536004661</v>
+        <v>102.0966536023758</v>
       </c>
       <c r="E40">
-        <v>117.3361000636724</v>
+        <v>117.3361000643016</v>
       </c>
       <c r="F40">
-        <v>103.5216090353388</v>
+        <v>103.5216090367698</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1197,19 +1197,19 @@
         <v>2050</v>
       </c>
       <c r="B41">
-        <v>136.3895638416469</v>
+        <v>136.3895638382694</v>
       </c>
       <c r="C41">
-        <v>117.3443959062797</v>
+        <v>117.3443959064649</v>
       </c>
       <c r="D41">
-        <v>101.2345810542505</v>
+        <v>101.2345810591051</v>
       </c>
       <c r="E41">
-        <v>117.9001205487792</v>
+        <v>117.9001205488275</v>
       </c>
       <c r="F41">
-        <v>102.5671746755796</v>
+        <v>102.5671746804345</v>
       </c>
     </row>
   </sheetData>
@@ -1267,19 +1267,19 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.1452793956164414</v>
+        <v>0.1452794114198362</v>
       </c>
       <c r="C3">
-        <v>0.1450830560053418</v>
+        <v>0.145083071787379</v>
       </c>
       <c r="D3">
-        <v>0.1450830560053417</v>
+        <v>0.1450830717873791</v>
       </c>
       <c r="E3">
-        <v>0.1450751748406989</v>
+        <v>0.1450751906227616</v>
       </c>
       <c r="F3">
-        <v>0.1450620395662928</v>
+        <v>0.1450620553483992</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1287,19 +1287,19 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.1816369129819771</v>
+        <v>0.181636899529273</v>
       </c>
       <c r="C4">
-        <v>0.1813914649141057</v>
+        <v>0.181391451479582</v>
       </c>
       <c r="D4">
-        <v>0.1813915105032801</v>
+        <v>0.1813914970687564</v>
       </c>
       <c r="E4">
-        <v>0.1813655109402137</v>
+        <v>0.1813654975057351</v>
       </c>
       <c r="F4">
-        <v>0.1813222634352978</v>
+        <v>0.1813222500008942</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1307,19 +1307,19 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.2371403903786543</v>
+        <v>0.2371404008424781</v>
       </c>
       <c r="C5">
-        <v>0.2368202188424889</v>
+        <v>0.2368202292921714</v>
       </c>
       <c r="D5">
-        <v>0.2368207435861525</v>
+        <v>0.2368207540358325</v>
       </c>
       <c r="E5">
-        <v>0.2367378257991327</v>
+        <v>0.2367378362489831</v>
       </c>
       <c r="F5">
-        <v>0.2366006090230814</v>
+        <v>0.2366006194732105</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1327,19 +1327,19 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.3260461147306919</v>
+        <v>0.3260461146391306</v>
       </c>
       <c r="C6">
-        <v>0.3256078832961355</v>
+        <v>0.325607883204691</v>
       </c>
       <c r="D6">
-        <v>0.3256118990553666</v>
+        <v>0.3256118989639122</v>
       </c>
       <c r="E6">
-        <v>0.3253542952216261</v>
+        <v>0.3253542951306557</v>
       </c>
       <c r="F6">
-        <v>0.3249324518807259</v>
+        <v>0.3249324517905448</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1347,19 +1347,19 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.4739438218527361</v>
+        <v>0.4739438216727918</v>
       </c>
       <c r="C7">
-        <v>0.4733184264858693</v>
+        <v>0.4733184263061309</v>
       </c>
       <c r="D7">
-        <v>0.4733436630161983</v>
+        <v>0.4733436628363967</v>
       </c>
       <c r="E7">
-        <v>0.4725627103812226</v>
+        <v>0.4725627102028335</v>
       </c>
       <c r="F7">
-        <v>0.4713082355760977</v>
+        <v>0.471308235399943</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1367,19 +1367,19 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.7257883745591727</v>
+        <v>0.7257883742173169</v>
       </c>
       <c r="C8">
-        <v>0.724890556918471</v>
+        <v>0.7248905565768804</v>
       </c>
       <c r="D8">
-        <v>0.7250292651307177</v>
+        <v>0.7250292647888065</v>
       </c>
       <c r="E8">
-        <v>0.7227231211345477</v>
+        <v>0.7227231207966281</v>
       </c>
       <c r="F8">
-        <v>0.7191385306889194</v>
+        <v>0.7191385303570473</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1387,19 +1387,19 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>1.157953982833573</v>
+        <v>1.157953982210619</v>
       </c>
       <c r="C9">
-        <v>1.15679684371191</v>
+        <v>1.156796843088892</v>
       </c>
       <c r="D9">
-        <v>1.157478445028275</v>
+        <v>1.157478444403732</v>
       </c>
       <c r="E9">
-        <v>1.150869114360562</v>
+        <v>1.150869113746959</v>
       </c>
       <c r="F9">
-        <v>1.14112654003483</v>
+        <v>1.141126539436616</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1407,19 +1407,19 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>1.893714521149819</v>
+        <v>1.8937145200725</v>
       </c>
       <c r="C10">
-        <v>1.892956759772216</v>
+        <v>1.89295675869254</v>
       </c>
       <c r="D10">
-        <v>1.895971177372823</v>
+        <v>1.895971176286781</v>
       </c>
       <c r="E10">
-        <v>1.877662403548862</v>
+        <v>1.877662402491697</v>
       </c>
       <c r="F10">
-        <v>1.85278062674236</v>
+        <v>1.852780625721431</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1427,19 +1427,19 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>3.117384905151875</v>
+        <v>3.117384903408206</v>
       </c>
       <c r="C11">
-        <v>3.120336244743424</v>
+        <v>3.12033624298789</v>
       </c>
       <c r="D11">
-        <v>3.132340934562783</v>
+        <v>3.132340932783336</v>
       </c>
       <c r="E11">
-        <v>3.083503954228273</v>
+        <v>3.083503952522073</v>
       </c>
       <c r="F11">
-        <v>3.024563279475314</v>
+        <v>3.024563277846492</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1447,19 +1447,19 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>5.075886168001927</v>
+        <v>5.075886165411384</v>
       </c>
       <c r="C12">
-        <v>5.094626071819436</v>
+        <v>5.094626069184797</v>
       </c>
       <c r="D12">
-        <v>5.137600074554873</v>
+        <v>5.137600071840263</v>
       </c>
       <c r="E12">
-        <v>5.012611066648307</v>
+        <v>5.012611064111384</v>
       </c>
       <c r="F12">
-        <v>4.884810071837583</v>
+        <v>4.884810069446964</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1467,19 +1467,19 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>8.050410223640499</v>
+        <v>8.050410220214424</v>
       </c>
       <c r="C13">
-        <v>8.121500972085808</v>
+        <v>8.121500968523179</v>
       </c>
       <c r="D13">
-        <v>8.25943786153084</v>
+        <v>8.259437857730237</v>
       </c>
       <c r="E13">
-        <v>7.953808860061036</v>
+        <v>7.95380885667039</v>
       </c>
       <c r="F13">
-        <v>7.70353582696897</v>
+        <v>7.703535823814508</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1487,19 +1487,19 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>12.28034780850724</v>
+        <v>12.28034780470608</v>
       </c>
       <c r="C14">
-        <v>12.49825878655826</v>
+        <v>12.49825878239236</v>
       </c>
       <c r="D14">
-        <v>12.89415517409696</v>
+        <v>12.89415516930483</v>
       </c>
       <c r="E14">
-        <v>12.18435798551051</v>
+        <v>12.18435798160953</v>
       </c>
       <c r="F14">
-        <v>11.74792724297646</v>
+        <v>11.74792723937957</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1507,19 +1507,19 @@
         <v>2024</v>
       </c>
       <c r="B15">
-        <v>17.84594559111853</v>
+        <v>17.84594558812026</v>
       </c>
       <c r="C15">
-        <v>18.41929530688393</v>
+        <v>18.41929530303994</v>
       </c>
       <c r="D15">
-        <v>19.43231398248635</v>
+        <v>19.43231397719486</v>
       </c>
       <c r="E15">
-        <v>17.8797256794794</v>
+        <v>17.87972567598781</v>
       </c>
       <c r="F15">
-        <v>17.21271573872828</v>
+        <v>17.21271573549115</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1527,19 +1527,19 @@
         <v>2025</v>
       </c>
       <c r="B16">
-        <v>24.56353494582056</v>
+        <v>24.56353494556669</v>
       </c>
       <c r="C16">
-        <v>25.88092575914292</v>
+        <v>25.88092575719385</v>
       </c>
       <c r="D16">
-        <v>28.18419158231252</v>
+        <v>28.18419157744953</v>
       </c>
       <c r="E16">
-        <v>25.01968982532882</v>
+        <v>25.01968982378331</v>
       </c>
       <c r="F16">
-        <v>24.14327086015191</v>
+        <v>24.14327085856811</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1547,19 +1547,19 @@
         <v>2026</v>
       </c>
       <c r="B17">
-        <v>32.00223673392776</v>
+        <v>32.00223673862452</v>
       </c>
       <c r="C17">
-        <v>34.65648513080038</v>
+        <v>34.65648513259584</v>
       </c>
       <c r="D17">
-        <v>39.29257284758152</v>
+        <v>39.29257284433492</v>
       </c>
       <c r="E17">
-        <v>33.35557660918591</v>
+        <v>33.35557661139037</v>
       </c>
       <c r="F17">
-        <v>32.38954861233844</v>
+        <v>32.38954861390461</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1567,19 +1567,19 @@
         <v>2027</v>
       </c>
       <c r="B18">
-        <v>39.7073232823016</v>
+        <v>39.70732329325847</v>
       </c>
       <c r="C18">
-        <v>44.39283178307811</v>
+        <v>44.39283178989366</v>
       </c>
       <c r="D18">
-        <v>52.62223088347217</v>
+        <v>52.62223088294729</v>
       </c>
       <c r="E18">
-        <v>42.49607210680289</v>
+        <v>42.49607211401983</v>
       </c>
       <c r="F18">
-        <v>41.62951398506693</v>
+        <v>41.62951399086554</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1587,19 +1587,19 @@
         <v>2028</v>
       </c>
       <c r="B19">
-        <v>47.5392588975297</v>
+        <v>47.53925891380706</v>
       </c>
       <c r="C19">
-        <v>54.76905994509821</v>
+        <v>54.76905995668197</v>
       </c>
       <c r="D19">
-        <v>67.60718164387158</v>
+        <v>67.60718164682783</v>
       </c>
       <c r="E19">
-        <v>52.07875008820236</v>
+        <v>52.07875010020467</v>
       </c>
       <c r="F19">
-        <v>51.45700670433483</v>
+        <v>51.45700671432595</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1607,19 +1607,19 @@
         <v>2029</v>
       </c>
       <c r="B20">
-        <v>55.82731637040401</v>
+        <v>55.82731638831743</v>
       </c>
       <c r="C20">
-        <v>65.55749933484257</v>
+        <v>65.55749934908935</v>
       </c>
       <c r="D20">
-        <v>83.11793658737632</v>
+        <v>83.11793659427777</v>
       </c>
       <c r="E20">
-        <v>61.885069535516</v>
+        <v>61.88506955018657</v>
       </c>
       <c r="F20">
-        <v>61.4705160916881</v>
+        <v>61.47051610438919</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1627,19 +1627,19 @@
         <v>2030</v>
       </c>
       <c r="B21">
-        <v>65.11720347360615</v>
+        <v>65.11720348787973</v>
       </c>
       <c r="C21">
-        <v>76.52914543480438</v>
+        <v>76.52914544851072</v>
       </c>
       <c r="D21">
-        <v>97.56994164334024</v>
+        <v>97.56994165459496</v>
       </c>
       <c r="E21">
-        <v>71.80188706023829</v>
+        <v>71.80188707421974</v>
       </c>
       <c r="F21">
-        <v>71.3223708111928</v>
+        <v>71.32237082409368</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1647,19 +1647,19 @@
         <v>2031</v>
       </c>
       <c r="B22">
-        <v>75.66094315505545</v>
+        <v>75.66094316116725</v>
       </c>
       <c r="C22">
-        <v>87.33242207077579</v>
+        <v>87.33242208104889</v>
       </c>
       <c r="D22">
-        <v>109.4121421110376</v>
+        <v>109.4121421269642</v>
       </c>
       <c r="E22">
-        <v>81.68590869115215</v>
+        <v>81.68590870126808</v>
       </c>
       <c r="F22">
-        <v>80.72502806943601</v>
+        <v>80.72502807995365</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1667,19 +1667,19 @@
         <v>2032</v>
       </c>
       <c r="B23">
-        <v>87.0893963400008</v>
+        <v>87.08939633620051</v>
       </c>
       <c r="C23">
-        <v>97.52337708016728</v>
+        <v>97.52337708549615</v>
       </c>
       <c r="D23">
-        <v>117.7855160809072</v>
+        <v>117.7855161011955</v>
       </c>
       <c r="E23">
-        <v>91.29380091488656</v>
+        <v>91.29380091933889</v>
       </c>
       <c r="F23">
-        <v>89.45137278533272</v>
+        <v>89.45137279172025</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1687,19 +1687,19 @@
         <v>2033</v>
       </c>
       <c r="B24">
-        <v>98.52266938619343</v>
+        <v>98.52266937397127</v>
       </c>
       <c r="C24">
-        <v>106.7348506825976</v>
+        <v>106.7348506829906</v>
       </c>
       <c r="D24">
-        <v>122.8959767933791</v>
+        <v>122.8959768164437</v>
       </c>
       <c r="E24">
-        <v>100.3360371634237</v>
+        <v>100.3360371621139</v>
       </c>
       <c r="F24">
-        <v>97.35280892561859</v>
+        <v>97.35280892732357</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1707,19 +1707,19 @@
         <v>2034</v>
       </c>
       <c r="B25">
-        <v>108.9469920629921</v>
+        <v>108.9469920460467</v>
       </c>
       <c r="C25">
-        <v>114.7977955400795</v>
+        <v>114.7977955365071</v>
       </c>
       <c r="D25">
-        <v>125.8337064216458</v>
+        <v>125.8337064445236</v>
       </c>
       <c r="E25">
-        <v>108.5582520281031</v>
+        <v>108.5582520222005</v>
       </c>
       <c r="F25">
-        <v>104.365391619973</v>
+        <v>104.3653916174618</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1727,19 +1727,19 @@
         <v>2035</v>
       </c>
       <c r="B26">
-        <v>117.557604191298</v>
+        <v>117.5576041739363</v>
       </c>
       <c r="C26">
-        <v>121.7182406242539</v>
+        <v>121.7182406180197</v>
       </c>
       <c r="D26">
-        <v>128.0139875257618</v>
+        <v>128.0139875448057</v>
       </c>
       <c r="E26">
-        <v>115.7751724695586</v>
+        <v>115.7751724608229</v>
       </c>
       <c r="F26">
-        <v>110.489412340015</v>
+        <v>110.4894123343761</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1747,19 +1747,19 @@
         <v>2036</v>
       </c>
       <c r="B27">
-        <v>123.9162698662939</v>
+        <v>123.9162698521243</v>
       </c>
       <c r="C27">
-        <v>127.5663458367244</v>
+        <v>127.5663458291173</v>
       </c>
       <c r="D27">
-        <v>130.6114974256484</v>
+        <v>130.6114974376622</v>
       </c>
       <c r="E27">
-        <v>121.8599225428602</v>
+        <v>121.8599225331295</v>
       </c>
       <c r="F27">
-        <v>115.7497529735687</v>
+        <v>115.7497529661136</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1767,19 +1767,19 @@
         <v>2037</v>
       </c>
       <c r="B28">
-        <v>127.9598570982844</v>
+        <v>127.9598570895414</v>
       </c>
       <c r="C28">
-        <v>132.3940581164518</v>
+        <v>132.3940581086483</v>
       </c>
       <c r="D28">
-        <v>134.2550035906513</v>
+        <v>134.2550035938606</v>
       </c>
       <c r="E28">
-        <v>126.7376653119344</v>
+        <v>126.7376653028237</v>
       </c>
       <c r="F28">
-        <v>120.1713620859976</v>
+        <v>120.1713620780043</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1787,19 +1787,19 @@
         <v>2038</v>
       </c>
       <c r="B29">
-        <v>129.935885203364</v>
+        <v>129.9358852007719</v>
       </c>
       <c r="C29">
-        <v>136.2251011948603</v>
+        <v>136.2251011878905</v>
       </c>
       <c r="D29">
-        <v>139.0132438714836</v>
+        <v>139.0132438659223</v>
       </c>
       <c r="E29">
-        <v>130.3990343017911</v>
+        <v>130.3990342945162</v>
       </c>
       <c r="F29">
-        <v>123.7811727216468</v>
+        <v>123.7811727141794</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1807,19 +1807,19 @@
         <v>2039</v>
       </c>
       <c r="B30">
-        <v>130.3174645947398</v>
+        <v>130.3174645977118</v>
       </c>
       <c r="C30">
-        <v>139.0969677399382</v>
+        <v>139.0969677346053</v>
       </c>
       <c r="D30">
-        <v>144.5653005330902</v>
+        <v>144.5653005203785</v>
       </c>
       <c r="E30">
-        <v>132.9232539867151</v>
+        <v>132.9232539819846</v>
       </c>
       <c r="F30">
-        <v>126.6310367893495</v>
+        <v>126.6310367831529</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1827,19 +1827,19 @@
         <v>2040</v>
       </c>
       <c r="B31">
-        <v>129.6989653333128</v>
+        <v>129.6989653403162</v>
       </c>
       <c r="C31">
-        <v>141.0950340516833</v>
+        <v>141.0950340484579</v>
       </c>
       <c r="D31">
-        <v>150.4081406640857</v>
+        <v>150.4081406468167</v>
       </c>
       <c r="E31">
-        <v>134.4749505203866</v>
+        <v>134.4749505183729</v>
       </c>
       <c r="F31">
-        <v>128.8062560691974</v>
+        <v>128.8062560646458</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1847,19 +1847,19 @@
         <v>2041</v>
       </c>
       <c r="B32">
-        <v>128.6915392266613</v>
+        <v>128.6915392356644</v>
       </c>
       <c r="C32">
-        <v>142.3642663588894</v>
+        <v>142.364266357851</v>
       </c>
       <c r="D32">
-        <v>156.0285872449234</v>
+        <v>156.0285872259703</v>
       </c>
       <c r="E32">
-        <v>135.2817113757305</v>
+        <v>135.2817113761441</v>
       </c>
       <c r="F32">
-        <v>130.4220205629971</v>
+        <v>130.4220205601315</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1867,19 +1867,19 @@
         <v>2042</v>
       </c>
       <c r="B33">
-        <v>127.8238196671548</v>
+        <v>127.8238196760824</v>
       </c>
       <c r="C33">
-        <v>143.0915946799305</v>
+        <v>143.0915946807956</v>
       </c>
       <c r="D33">
-        <v>161.0057341202847</v>
+        <v>161.0057341022487</v>
       </c>
       <c r="E33">
-        <v>135.5954581562051</v>
+        <v>135.5954581584355</v>
       </c>
       <c r="F33">
-        <v>131.603162608368</v>
+        <v>131.603162606996</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1887,19 +1887,19 @@
         <v>2043</v>
       </c>
       <c r="B34">
-        <v>127.4670597958154</v>
+        <v>127.467059802948</v>
       </c>
       <c r="C34">
-        <v>143.4759245841045</v>
+        <v>143.4759245863392</v>
       </c>
       <c r="D34">
-        <v>165.0552604277464</v>
+        <v>165.0552604126212</v>
       </c>
       <c r="E34">
-        <v>135.6553332408127</v>
+        <v>135.655333244106</v>
       </c>
       <c r="F34">
-        <v>132.4622198677665</v>
+        <v>132.4622198675908</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1907,19 +1907,19 @@
         <v>2044</v>
       </c>
       <c r="B35">
-        <v>127.7952886377703</v>
+        <v>127.795288642025</v>
       </c>
       <c r="C35">
-        <v>143.6972086037316</v>
+        <v>143.6972086067001</v>
       </c>
       <c r="D35">
-        <v>168.0326483932837</v>
+        <v>168.0326483823326</v>
       </c>
       <c r="E35">
-        <v>135.6584791533814</v>
+        <v>135.6584791569977</v>
       </c>
       <c r="F35">
-        <v>133.0839039726692</v>
+        <v>133.083903973393</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1927,19 +1927,19 @@
         <v>2045</v>
       </c>
       <c r="B36">
-        <v>128.791362678857</v>
+        <v>128.7913626799032</v>
       </c>
       <c r="C36">
-        <v>143.8985167669133</v>
+        <v>143.8985167700104</v>
       </c>
       <c r="D36">
-        <v>169.9188963132981</v>
+        <v>169.9188963070746</v>
       </c>
       <c r="E36">
-        <v>135.7466940360103</v>
+        <v>135.7466940393388</v>
       </c>
       <c r="F36">
-        <v>133.5259035759199</v>
+        <v>133.525903577302</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1947,19 +1947,19 @@
         <v>2046</v>
       </c>
       <c r="B37">
-        <v>130.2890102103233</v>
+        <v>130.2890102085246</v>
       </c>
       <c r="C37">
-        <v>144.1782212650096</v>
+        <v>144.1782212677523</v>
       </c>
       <c r="D37">
-        <v>170.7960269997642</v>
+        <v>170.7960269982123</v>
       </c>
       <c r="E37">
-        <v>136.0034073052039</v>
+        <v>136.0034073078218</v>
       </c>
       <c r="F37">
-        <v>133.8276597801998</v>
+        <v>133.8276597820548</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1967,19 +1967,19 @@
         <v>2047</v>
       </c>
       <c r="B38">
-        <v>132.0370451218019</v>
+        <v>132.0370451180287</v>
       </c>
       <c r="C38">
-        <v>144.5900700824588</v>
+        <v>144.5900700845323</v>
       </c>
       <c r="D38">
-        <v>170.8192689615816</v>
+        <v>170.8192689641773</v>
       </c>
       <c r="E38">
-        <v>136.4582401989542</v>
+        <v>136.458240200643</v>
       </c>
       <c r="F38">
-        <v>134.0212881616916</v>
+        <v>134.021288163871</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1987,19 +1987,19 @@
         <v>2048</v>
       </c>
       <c r="B39">
-        <v>133.7692167127189</v>
+        <v>133.7692167080786</v>
       </c>
       <c r="C39">
-        <v>145.1489111911845</v>
+        <v>145.1489111924413</v>
       </c>
       <c r="D39">
-        <v>170.1907484313786</v>
+        <v>170.1907484372711</v>
       </c>
       <c r="E39">
-        <v>137.097220139302</v>
+        <v>137.0972201400273</v>
       </c>
       <c r="F39">
-        <v>134.140226646982</v>
+        <v>134.1402266493379</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2007,19 +2007,19 @@
         <v>2049</v>
       </c>
       <c r="B40">
-        <v>135.2657387848821</v>
+        <v>135.2657387804554</v>
       </c>
       <c r="C40">
-        <v>145.8414932986245</v>
+        <v>145.8414932990678</v>
       </c>
       <c r="D40">
-        <v>169.1386119762718</v>
+        <v>169.1386119844234</v>
       </c>
       <c r="E40">
-        <v>137.8783078152333</v>
+        <v>137.8783078151103</v>
       </c>
       <c r="F40">
-        <v>134.2251407840392</v>
+        <v>134.225140786416</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2027,19 +2027,19 @@
         <v>2050</v>
       </c>
       <c r="B41">
-        <v>136.3895638416469</v>
+        <v>136.3895638382694</v>
       </c>
       <c r="C41">
-        <v>146.6343865571677</v>
+        <v>146.6343865569119</v>
       </c>
       <c r="D41">
-        <v>167.8956200397908</v>
+        <v>167.8956200490957</v>
       </c>
       <c r="E41">
-        <v>138.7437002762786</v>
+        <v>138.743700275515</v>
       </c>
       <c r="F41">
-        <v>134.3209748185346</v>
+        <v>134.32097482076</v>
       </c>
     </row>
   </sheetData>
@@ -2097,7 +2097,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.0001963396110995197</v>
+        <v>0.0001963396324572107</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2117,19 +2117,19 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.0004833169385966783</v>
+        <v>0.0004833169462880981</v>
       </c>
       <c r="C4">
-        <v>0.0001647747362880995</v>
+        <v>0.0001647747544398585</v>
       </c>
       <c r="D4">
-        <v>0.0001647747362881</v>
+        <v>0.0001647747544398585</v>
       </c>
       <c r="E4">
-        <v>4.684205771923339e-05</v>
+        <v>4.68420629908969E-05</v>
       </c>
       <c r="F4">
-        <v>4.684205771923339e-05</v>
+        <v>4.68420629908969E-05</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2137,19 +2137,19 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.001090113337723234</v>
+        <v>0.001090113381213352</v>
       </c>
       <c r="C5">
-        <v>0.000531440032632321</v>
+        <v>0.0005314400532733396</v>
       </c>
       <c r="D5">
-        <v>0.0005314400441780434</v>
+        <v>0.0005314400648190609</v>
       </c>
       <c r="E5">
-        <v>0.0001507315567569929</v>
+        <v>0.0001507315628341516</v>
       </c>
       <c r="F5">
-        <v>0.0001507315593101926</v>
+        <v>0.0001507315653873514</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2157,19 +2157,19 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.002301265660979809</v>
+        <v>0.002301265730193032</v>
       </c>
       <c r="C6">
-        <v>0.001279890836474212</v>
+        <v>0.001279890885297282</v>
       </c>
       <c r="D6">
-        <v>0.001279890990513036</v>
+        <v>0.001279891039336104</v>
       </c>
       <c r="E6">
-        <v>0.0003623271950454599</v>
+        <v>0.0003623272095269199</v>
       </c>
       <c r="F6">
-        <v>0.0003623272291514769</v>
+        <v>0.0003623272436329367</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2177,19 +2177,19 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.004597339085475379</v>
+        <v>0.00459733920598419</v>
       </c>
       <c r="C7">
-        <v>0.002709508873345587</v>
+        <v>0.002709508958596605</v>
       </c>
       <c r="D7">
-        <v>0.002709510164156485</v>
+        <v>0.002709510249407495</v>
       </c>
       <c r="E7">
-        <v>0.0007659001162499203</v>
+        <v>0.0007659001419454006</v>
       </c>
       <c r="F7">
-        <v>0.0007659004023947119</v>
+        <v>0.0007659004280901914</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2197,19 +2197,19 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.008755648865133017</v>
+        <v>0.008755649062821917</v>
       </c>
       <c r="C8">
-        <v>0.005294667661864786</v>
+        <v>0.005294667802272036</v>
       </c>
       <c r="D8">
-        <v>0.005294676271172933</v>
+        <v>0.005294676411580155</v>
       </c>
       <c r="E8">
-        <v>0.00149481617873025</v>
+        <v>0.001494816222001492</v>
       </c>
       <c r="F8">
-        <v>0.001494818089563099</v>
+        <v>0.001494818132834335</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2217,19 +2217,19 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.01599415621741926</v>
+        <v>0.0159941565230986</v>
       </c>
       <c r="C9">
-        <v>0.009759690463027507</v>
+        <v>0.009759690681337981</v>
       </c>
       <c r="D9">
-        <v>0.009759739843516428</v>
+        <v>0.009759740061826781</v>
       </c>
       <c r="E9">
-        <v>0.00275186252203943</v>
+        <v>0.002751862591401143</v>
       </c>
       <c r="F9">
-        <v>0.002751873496671056</v>
+        <v>0.00275187356603274</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2237,19 +2237,19 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.02818496063301321</v>
+        <v>0.02818496107861729</v>
       </c>
       <c r="C10">
-        <v>0.01718690986445879</v>
+        <v>0.01718691018515776</v>
       </c>
       <c r="D10">
-        <v>0.01718716104741061</v>
+        <v>0.017187161368109</v>
       </c>
       <c r="E10">
-        <v>0.004836967866012867</v>
+        <v>0.004836967972193126</v>
       </c>
       <c r="F10">
-        <v>0.004837023778931492</v>
+        <v>0.004837023885111626</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2257,19 +2257,19 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.04818186364036228</v>
+        <v>0.04818186425255487</v>
       </c>
       <c r="C11">
-        <v>0.02918562210552873</v>
+        <v>0.02918562255085464</v>
       </c>
       <c r="D11">
-        <v>0.02918676918568981</v>
+        <v>0.02918676963101325</v>
       </c>
       <c r="E11">
-        <v>0.008187561824161513</v>
+        <v>0.008187561979914375</v>
       </c>
       <c r="F11">
-        <v>0.008187817678346858</v>
+        <v>0.008187817834099165</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2277,19 +2277,19 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.08032602556128543</v>
+        <v>0.08032602635299271</v>
       </c>
       <c r="C12">
-        <v>0.04816832694213758</v>
+        <v>0.04816832752666401</v>
       </c>
       <c r="D12">
-        <v>0.04817304952536403</v>
+        <v>0.0481730501098808</v>
       </c>
       <c r="E12">
-        <v>0.01344074836891514</v>
+        <v>0.01344074858852689</v>
       </c>
       <c r="F12">
-        <v>0.01344180460225851</v>
+        <v>0.0134418048218681</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2297,19 +2297,19 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.1312070139977763</v>
+        <v>0.1312070149591681</v>
       </c>
       <c r="C13">
-        <v>0.0777990175926085</v>
+        <v>0.07779901831725297</v>
       </c>
       <c r="D13">
-        <v>0.07781655938008596</v>
+        <v>0.07781656010469667</v>
       </c>
       <c r="E13">
-        <v>0.02153189759004521</v>
+        <v>0.02153189788845248</v>
       </c>
       <c r="F13">
-        <v>0.02153583583738078</v>
+        <v>0.02153583613578047</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2317,19 +2317,19 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.2107522675488965</v>
+        <v>0.2107522686403912</v>
       </c>
       <c r="C14">
-        <v>0.1236884871157186</v>
+        <v>0.123688487962672</v>
       </c>
       <c r="D14">
-        <v>0.1237472473488833</v>
+        <v>0.1237472481957308</v>
       </c>
       <c r="E14">
-        <v>0.03385191614168746</v>
+        <v>0.03385191653310763</v>
       </c>
       <c r="F14">
-        <v>0.03386517952030886</v>
+        <v>0.03386517991170507</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2337,19 +2337,19 @@
         <v>2024</v>
       </c>
       <c r="B15">
-        <v>0.3336982303562527</v>
+        <v>0.3336982315067402</v>
       </c>
       <c r="C15">
-        <v>0.1944004437337144</v>
+        <v>0.1944004446641972</v>
       </c>
       <c r="D15">
-        <v>0.1945778593539151</v>
+        <v>0.1945778602841008</v>
       </c>
       <c r="E15">
-        <v>0.05249489112902512</v>
+        <v>0.0524948916250211</v>
       </c>
       <c r="F15">
-        <v>0.05253524613230399</v>
+        <v>0.05253524662823211</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2357,19 +2357,19 @@
         <v>2025</v>
       </c>
       <c r="B16">
-        <v>0.5214550409716485</v>
+        <v>0.5214550420845162</v>
       </c>
       <c r="C16">
-        <v>0.3027927256701111</v>
+        <v>0.3027927266265873</v>
       </c>
       <c r="D16">
-        <v>0.3032756333813366</v>
+        <v>0.3032756343370654</v>
       </c>
       <c r="E16">
-        <v>0.08063744910908063</v>
+        <v>0.0806374497160412</v>
       </c>
       <c r="F16">
-        <v>0.08074848905658163</v>
+        <v>0.08074848966336909</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2377,19 +2377,19 @@
         <v>2026</v>
       </c>
       <c r="B17">
-        <v>0.8043134554807252</v>
+        <v>0.8043134564479778</v>
       </c>
       <c r="C17">
-        <v>0.4676457007857129</v>
+        <v>0.4676457016988838</v>
       </c>
       <c r="D17">
-        <v>0.4688323126525523</v>
+        <v>0.4688323135640382</v>
       </c>
       <c r="E17">
-        <v>0.1230932526036724</v>
+        <v>0.1230932533197669</v>
       </c>
       <c r="F17">
-        <v>0.1233702401865967</v>
+        <v>0.1233702409022933</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2397,19 +2397,19 @@
         <v>2027</v>
       </c>
       <c r="B18">
-        <v>1.223805655308896</v>
+        <v>1.22380565603052</v>
       </c>
       <c r="C18">
-        <v>0.715443045185118</v>
+        <v>0.715443045984089</v>
       </c>
       <c r="D18">
-        <v>0.7180838866815085</v>
+        <v>0.718083887477063</v>
       </c>
       <c r="E18">
-        <v>0.1870732522756712</v>
+        <v>0.1870732530874874</v>
       </c>
       <c r="F18">
-        <v>0.1877023933600007</v>
+        <v>0.187702394170988</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2417,19 +2417,19 @@
         <v>2028</v>
       </c>
       <c r="B19">
-        <v>1.8347484617175</v>
+        <v>1.834748462121342</v>
       </c>
       <c r="C19">
-        <v>1.082081246226928</v>
+        <v>1.082081246849641</v>
       </c>
       <c r="D19">
-        <v>1.087434453965534</v>
+        <v>1.087434454581981</v>
       </c>
       <c r="E19">
-        <v>0.2831517306723034</v>
+        <v>0.283151731551695</v>
       </c>
       <c r="F19">
-        <v>0.2844616992948655</v>
+        <v>0.2844617001726797</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2437,19 +2437,19 @@
         <v>2029</v>
       </c>
       <c r="B20">
-        <v>2.706137362035793</v>
+        <v>2.706137362094124</v>
       </c>
       <c r="C20">
-        <v>1.614175902062405</v>
+        <v>1.614175902463888</v>
       </c>
       <c r="D20">
-        <v>1.624140122734758</v>
+        <v>1.624140123125748</v>
       </c>
       <c r="E20">
-        <v>0.426398839546092</v>
+        <v>0.4263988404481999</v>
       </c>
       <c r="F20">
-        <v>0.429038346011486</v>
+        <v>0.4290383469115601</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2457,19 +2457,19 @@
         <v>2030</v>
       </c>
       <c r="B21">
-        <v>3.919965033173844</v>
+        <v>3.919965032915314</v>
       </c>
       <c r="C21">
-        <v>2.369499947378027</v>
+        <v>2.369499947535975</v>
       </c>
       <c r="D21">
-        <v>2.386798516364973</v>
+        <v>2.38679851650789</v>
       </c>
       <c r="E21">
-        <v>0.6376125178731167</v>
+        <v>0.6376125187367196</v>
       </c>
       <c r="F21">
-        <v>0.6433076416767254</v>
+        <v>0.6433076425346802</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2477,19 +2477,19 @@
         <v>2031</v>
       </c>
       <c r="B22">
-        <v>5.567414416908105</v>
+        <v>5.567414416425306</v>
       </c>
       <c r="C22">
-        <v>3.4160356484798</v>
+        <v>3.416035648398747</v>
       </c>
       <c r="D22">
-        <v>3.44467930783918</v>
+        <v>3.444679307737983</v>
       </c>
       <c r="E22">
-        <v>0.9445758372218233</v>
+        <v>0.944575837972772</v>
       </c>
       <c r="F22">
-        <v>0.9575058380212809</v>
+        <v>0.9575058387493004</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2497,19 +2497,19 @@
         <v>2032</v>
       </c>
       <c r="B23">
-        <v>7.742579794517445</v>
+        <v>7.742579793969218</v>
       </c>
       <c r="C23">
-        <v>4.829225060546694</v>
+        <v>4.829225060262043</v>
       </c>
       <c r="D23">
-        <v>4.874611739214672</v>
+        <v>4.874611738899082</v>
       </c>
       <c r="E23">
-        <v>1.383225196645756</v>
+        <v>1.383225197203275</v>
       </c>
       <c r="F23">
-        <v>1.410093697669441</v>
+        <v>1.410093698176862</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2517,19 +2517,19 @@
         <v>2033</v>
       </c>
       <c r="B24">
-        <v>10.53445490911846</v>
+        <v>10.53445490872406</v>
       </c>
       <c r="C24">
-        <v>6.687267569123104</v>
+        <v>6.68726756870469</v>
       </c>
       <c r="D24">
-        <v>6.755572166468383</v>
+        <v>6.755572166003817</v>
       </c>
       <c r="E24">
-        <v>1.998500544934044</v>
+        <v>1.998500545218786</v>
       </c>
       <c r="F24">
-        <v>2.046156321699176</v>
+        <v>2.046156321907522</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2537,19 +2537,19 @@
         <v>2034</v>
       </c>
       <c r="B25">
-        <v>14.01825004568209</v>
+        <v>14.01825004570292</v>
       </c>
       <c r="C25">
-        <v>9.064642997797787</v>
+        <v>9.064642997350793</v>
       </c>
       <c r="D25">
-        <v>9.161784890748187</v>
+        <v>9.161784890240568</v>
       </c>
       <c r="E25">
-        <v>2.844509091878764</v>
+        <v>2.844509091821164</v>
       </c>
       <c r="F25">
-        <v>2.917567381554761</v>
+        <v>2.917567381408164</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2557,19 +2557,19 @@
         <v>2035</v>
       </c>
       <c r="B26">
-        <v>18.2473475798315</v>
+        <v>18.24734758053705</v>
       </c>
       <c r="C26">
-        <v>12.02437064563936</v>
+        <v>12.02437064529974</v>
       </c>
       <c r="D26">
-        <v>12.15483514211479</v>
+        <v>12.15483514170767</v>
       </c>
       <c r="E26">
-        <v>3.98356898737205</v>
+        <v>3.983568986919932</v>
       </c>
       <c r="F26">
-        <v>4.083414264742795</v>
+        <v>4.083414264207891</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2577,19 +2577,19 @@
         <v>2036</v>
       </c>
       <c r="B27">
-        <v>23.24726386400471</v>
+        <v>23.24726386562212</v>
       </c>
       <c r="C27">
-        <v>15.60987948533893</v>
+        <v>15.60987948526103</v>
       </c>
       <c r="D27">
-        <v>15.77590956290674</v>
+        <v>15.77590956276834</v>
       </c>
       <c r="E27">
-        <v>5.483766257844632</v>
+        <v>5.483766256969719</v>
       </c>
       <c r="F27">
-        <v>5.608584504610736</v>
+        <v>5.608584503679053</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2597,19 +2597,19 @@
         <v>2037</v>
       </c>
       <c r="B28">
-        <v>29.01261176958204</v>
+        <v>29.0126117722344</v>
       </c>
       <c r="C28">
-        <v>19.83767681984053</v>
+        <v>19.8376768201766</v>
       </c>
       <c r="D28">
-        <v>20.03867077359575</v>
+        <v>20.03867077389404</v>
       </c>
       <c r="E28">
-        <v>7.414818277535678</v>
+        <v>7.414818276239322</v>
       </c>
       <c r="F28">
-        <v>7.560961385203323</v>
+        <v>7.560961383888903</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2617,19 +2617,19 @@
         <v>2038</v>
       </c>
       <c r="B29">
-        <v>35.50713082352723</v>
+        <v>35.50713082717284</v>
       </c>
       <c r="C29">
-        <v>24.69211481669616</v>
+        <v>24.69211481756996</v>
       </c>
       <c r="D29">
-        <v>24.92473298825618</v>
+        <v>24.92473298912924</v>
       </c>
       <c r="E29">
-        <v>9.842238757297729</v>
+        <v>9.842238755616389</v>
       </c>
       <c r="F29">
-        <v>10.00669289247782</v>
+        <v>10.0066928908209</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2637,19 +2637,19 @@
         <v>2039</v>
       </c>
       <c r="B30">
-        <v>42.66569261570089</v>
+        <v>42.6656926200918</v>
       </c>
       <c r="C30">
-        <v>30.12332745237888</v>
+        <v>30.1233274538584</v>
       </c>
       <c r="D30">
-        <v>30.38250533236476</v>
+        <v>30.38250533388889</v>
       </c>
       <c r="E30">
-        <v>12.82001462148624</v>
+        <v>12.82001461949704</v>
       </c>
       <c r="F30">
-        <v>13.00345500806376</v>
+        <v>13.00345500612947</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2657,19 +2657,19 @@
         <v>2040</v>
       </c>
       <c r="B31">
-        <v>50.39633486731263</v>
+        <v>50.39633487199249</v>
       </c>
       <c r="C31">
-        <v>36.04887548884103</v>
+        <v>36.04887549091717</v>
       </c>
       <c r="D31">
-        <v>36.32951017348425</v>
+        <v>36.32951017565328</v>
       </c>
       <c r="E31">
-        <v>16.38225034362373</v>
+        <v>16.38225034144973</v>
       </c>
       <c r="F31">
-        <v>16.59132365683779</v>
+        <v>16.5913236547252</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -2677,19 +2677,19 @@
         <v>2041</v>
       </c>
       <c r="B32">
-        <v>58.58049334324549</v>
+        <v>58.58049334760061</v>
       </c>
       <c r="C32">
-        <v>42.35892911592038</v>
+        <v>42.35892911849807</v>
       </c>
       <c r="D32">
-        <v>42.65861512724278</v>
+        <v>42.65861512995598</v>
       </c>
       <c r="E32">
-        <v>20.53452718573322</v>
+        <v>20.53452718354721</v>
       </c>
       <c r="F32">
-        <v>20.78429285832381</v>
+        <v>20.78429285617301</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -2697,19 +2697,19 @@
         <v>2042</v>
       </c>
       <c r="B33">
-        <v>67.07089422914301</v>
+        <v>67.07089423250693</v>
       </c>
       <c r="C33">
-        <v>48.92418751197648</v>
+        <v>48.92418751488248</v>
       </c>
       <c r="D33">
-        <v>49.24582515441315</v>
+        <v>49.24582515748389</v>
       </c>
       <c r="E33">
-        <v>25.24607479464923</v>
+        <v>25.24607479267389</v>
       </c>
       <c r="F33">
-        <v>25.56087181095101</v>
+        <v>25.56087180895137</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -2717,19 +2717,19 @@
         <v>2043</v>
       </c>
       <c r="B34">
-        <v>75.68874345744879</v>
+        <v>75.68874345924212</v>
       </c>
       <c r="C34">
-        <v>55.60532361662931</v>
+        <v>55.60532361963615</v>
       </c>
       <c r="D34">
-        <v>55.95975411134694</v>
+        <v>55.95975411452874</v>
       </c>
       <c r="E34">
-        <v>30.44420176454611</v>
+        <v>30.44420176304796</v>
       </c>
       <c r="F34">
-        <v>30.85653678243418</v>
+        <v>30.85653678082562</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -2737,19 +2737,19 @@
         <v>2044</v>
       </c>
       <c r="B35">
-        <v>84.22385056457256</v>
+        <v>84.22385056444352</v>
       </c>
       <c r="C35">
-        <v>62.26263461955875</v>
+        <v>62.26263462242007</v>
       </c>
       <c r="D35">
-        <v>62.66970808630556</v>
+        <v>62.6697080893256</v>
       </c>
       <c r="E35">
-        <v>36.01266843711589</v>
+        <v>36.01266843639044</v>
       </c>
       <c r="F35">
-        <v>36.55944514811954</v>
+        <v>36.55944514718488</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -2757,19 +2757,19 @@
         <v>2045</v>
       </c>
       <c r="B36">
-        <v>92.44190277822254</v>
+        <v>92.44190277614734</v>
       </c>
       <c r="C36">
-        <v>68.76472197180378</v>
+        <v>68.76472197429275</v>
       </c>
       <c r="D36">
-        <v>69.25129519941075</v>
+        <v>69.25129520201766</v>
       </c>
       <c r="E36">
-        <v>41.79563013117489</v>
+        <v>41.79563013152143</v>
       </c>
       <c r="F36">
-        <v>42.51223860584769</v>
+        <v>42.51223860589362</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2777,19 +2777,19 @@
         <v>2046</v>
       </c>
       <c r="B37">
-        <v>100.1014478619715</v>
+        <v>100.1014478582808</v>
       </c>
       <c r="C37">
-        <v>74.99534397005149</v>
+        <v>74.99534397199366</v>
       </c>
       <c r="D37">
-        <v>75.59011443571775</v>
+        <v>75.59011443771814</v>
       </c>
       <c r="E37">
-        <v>47.60824665099758</v>
+        <v>47.60824665268353</v>
       </c>
       <c r="F37">
-        <v>48.51978274734685</v>
+        <v>48.51978274867617</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2797,19 +2797,19 @@
         <v>2047</v>
       </c>
       <c r="B38">
-        <v>106.9796155115961</v>
+        <v>106.9796155069151</v>
       </c>
       <c r="C38">
-        <v>80.85798957807887</v>
+        <v>80.8579895793731</v>
       </c>
       <c r="D38">
-        <v>81.5839113036804</v>
+        <v>81.58391130496497</v>
       </c>
       <c r="E38">
-        <v>53.2539296688927</v>
+        <v>53.25392967211044</v>
       </c>
       <c r="F38">
-        <v>54.36599428743408</v>
+        <v>54.36599429029944</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2817,19 +2817,19 @@
         <v>2048</v>
       </c>
       <c r="B39">
-        <v>112.9016652874762</v>
+        <v>112.9016652825919</v>
       </c>
       <c r="C39">
-        <v>86.2781650166589</v>
+        <v>86.27816501728402</v>
       </c>
       <c r="D39">
-        <v>87.14515926389086</v>
+        <v>87.1451592644454</v>
       </c>
       <c r="E39">
-        <v>58.54657329617814</v>
+        <v>58.54657330100002</v>
       </c>
       <c r="F39">
-        <v>59.83924212854266</v>
+        <v>59.83924213308698</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -2837,19 +2837,19 @@
         <v>2049</v>
       </c>
       <c r="B40">
-        <v>117.7669663997275</v>
+        <v>117.7669663954195</v>
       </c>
       <c r="C40">
-        <v>91.20378467948387</v>
+        <v>91.2037846794924</v>
       </c>
       <c r="D40">
-        <v>92.2043887699439</v>
+        <v>92.20438876983998</v>
       </c>
       <c r="E40">
-        <v>63.3343544156429</v>
+        <v>63.33435442198325</v>
       </c>
       <c r="F40">
-        <v>64.76119930199019</v>
+        <v>64.76119930819986</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -2857,19 +2857,19 @@
         <v>2050</v>
       </c>
       <c r="B41">
-        <v>121.5642085708811</v>
+        <v>121.5642085677618</v>
       </c>
       <c r="C41">
-        <v>95.60430331601275</v>
+        <v>95.60430331551515</v>
       </c>
       <c r="D41">
-        <v>96.71365183120497</v>
+        <v>96.71365183058037</v>
       </c>
       <c r="E41">
-        <v>67.52041278797586</v>
+        <v>67.52041279556997</v>
       </c>
       <c r="F41">
-        <v>69.01363541211768</v>
+        <v>69.01363541977912</v>
       </c>
     </row>
   </sheetData>
@@ -2927,7 +2927,7 @@
         <v>2012</v>
       </c>
       <c r="B3">
-        <v>0.0001963396110995197</v>
+        <v>0.0001963396324572107</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2947,19 +2947,19 @@
         <v>2013</v>
       </c>
       <c r="B4">
-        <v>0.0004833169385966783</v>
+        <v>0.0004833169462880981</v>
       </c>
       <c r="C4">
-        <v>0.0002378656726444074</v>
+        <v>0.0002378656985165683</v>
       </c>
       <c r="D4">
-        <v>0.0002375286309269142</v>
+        <v>0.0002375286567646777</v>
       </c>
       <c r="E4">
-        <v>0.00023790593168398</v>
+        <v>0.000237905957556009</v>
       </c>
       <c r="F4">
-        <v>0.0002369751666724878</v>
+        <v>0.0002369751924528972</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2967,19 +2967,19 @@
         <v>2014</v>
       </c>
       <c r="B5">
-        <v>0.001090113337723234</v>
+        <v>0.001090113381213352</v>
       </c>
       <c r="C5">
-        <v>0.0007698868502696646</v>
+        <v>0.0007698868796175904</v>
       </c>
       <c r="D5">
-        <v>0.0007684358448801073</v>
+        <v>0.0007684358741589987</v>
       </c>
       <c r="E5">
-        <v>0.0007703199814066875</v>
+        <v>0.0007703200107533972</v>
       </c>
       <c r="F5">
-        <v>0.0007661066584163964</v>
+        <v>0.0007661066875799836</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2987,19 +2987,19 @@
         <v>2015</v>
       </c>
       <c r="B6">
-        <v>0.002301265660979809</v>
+        <v>0.002301265730193032</v>
       </c>
       <c r="C6">
-        <v>0.001862464418428537</v>
+        <v>0.001862464487760721</v>
       </c>
       <c r="D6">
-        <v>0.001857548157902343</v>
+        <v>0.00185754822703287</v>
       </c>
       <c r="E6">
-        <v>0.001865529862657588</v>
+        <v>0.0018655299319818</v>
       </c>
       <c r="F6">
-        <v>0.001849989451978082</v>
+        <v>0.001849989520770864</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -3007,19 +3007,19 @@
         <v>2016</v>
       </c>
       <c r="B7">
-        <v>0.004597339085475379</v>
+        <v>0.00459733920598419</v>
       </c>
       <c r="C7">
-        <v>0.00396742329720332</v>
+        <v>0.003967423417929323</v>
       </c>
       <c r="D7">
-        <v>0.003951895915512432</v>
+        <v>0.003951896035744761</v>
       </c>
       <c r="E7">
-        <v>0.003985117241954226</v>
+        <v>0.003985117362636833</v>
       </c>
       <c r="F7">
-        <v>0.003929722504337081</v>
+        <v>0.003929722623737491</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -3027,19 +3027,19 @@
         <v>2017</v>
       </c>
       <c r="B8">
-        <v>0.008755648865133017</v>
+        <v>0.008755649062821917</v>
       </c>
       <c r="C8">
-        <v>0.007828114659850617</v>
+        <v>0.007828114857877525</v>
       </c>
       <c r="D8">
-        <v>0.007779650955957802</v>
+        <v>0.007779651152871217</v>
       </c>
       <c r="E8">
-        <v>0.007917210340928266</v>
+        <v>0.007917210538748005</v>
       </c>
       <c r="F8">
-        <v>0.007717838211453335</v>
+        <v>0.007717838406466579</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -3047,19 +3047,19 @@
         <v>2018</v>
       </c>
       <c r="B9">
-        <v>0.01599415621741926</v>
+        <v>0.0159941565230986</v>
       </c>
       <c r="C9">
-        <v>0.01466941667231993</v>
+        <v>0.01466941697831231</v>
       </c>
       <c r="D9">
-        <v>0.01451613687474505</v>
+        <v>0.01451613717845647</v>
       </c>
       <c r="E9">
-        <v>0.0150710028769417</v>
+        <v>0.01507100318204951</v>
       </c>
       <c r="F9">
-        <v>0.01434805598156309</v>
+        <v>0.01434805628127938</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -3067,19 +3067,19 @@
         <v>2019</v>
       </c>
       <c r="B10">
-        <v>0.02818496063301321</v>
+        <v>0.02818496107861729</v>
       </c>
       <c r="C10">
-        <v>0.0266024135072033</v>
+        <v>0.02660241395223504</v>
       </c>
       <c r="D10">
-        <v>0.02611100243999932</v>
+        <v>0.02611100288089928</v>
       </c>
       <c r="E10">
-        <v>0.02823758587076847</v>
+        <v>0.02823758631240244</v>
       </c>
       <c r="F10">
-        <v>0.02565849629157077</v>
+        <v>0.02565849672482105</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -3087,19 +3087,19 @@
         <v>2020</v>
       </c>
       <c r="B11">
-        <v>0.04818186364036228</v>
+        <v>0.04818186425255487</v>
       </c>
       <c r="C11">
-        <v>0.0475610584568521</v>
+        <v>0.04756105906441329</v>
       </c>
       <c r="D11">
-        <v>0.0459943507868366</v>
+        <v>0.04599435138815652</v>
       </c>
       <c r="E11">
-        <v>0.0535853637729578</v>
+        <v>0.05358536436878836</v>
       </c>
       <c r="F11">
-        <v>0.04478535640408481</v>
+        <v>0.04478535699228051</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3107,19 +3107,19 @@
         <v>2021</v>
       </c>
       <c r="B12">
-        <v>0.08032602556128543</v>
+        <v>0.08032602635299271</v>
       </c>
       <c r="C12">
-        <v>0.08539211778654449</v>
+        <v>0.08539211856021781</v>
       </c>
       <c r="D12">
-        <v>0.08055909099451034</v>
+        <v>0.08055909176164616</v>
       </c>
       <c r="E12">
-        <v>0.1054400633495025</v>
+        <v>0.1054400640869167</v>
       </c>
       <c r="F12">
-        <v>0.07738936504108866</v>
+        <v>0.07738936578859107</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3127,19 +3127,19 @@
         <v>2022</v>
       </c>
       <c r="B13">
-        <v>0.1312070139977763</v>
+        <v>0.1312070149591681</v>
       </c>
       <c r="C13">
-        <v>0.1559589049374831</v>
+        <v>0.1559589058444819</v>
       </c>
       <c r="D13">
-        <v>0.1418961851696648</v>
+        <v>0.1418961860771698</v>
       </c>
       <c r="E13">
-        <v>0.2160544407129102</v>
+        <v>0.216054441520098</v>
       </c>
       <c r="F13">
-        <v>0.1339046760754996</v>
+        <v>0.1339046769587598</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3147,19 +3147,19 @@
         <v>2023</v>
       </c>
       <c r="B14">
-        <v>0.2107522675488965</v>
+        <v>0.2107522686403912</v>
       </c>
       <c r="C14">
-        <v>0.2896650694142907</v>
+        <v>0.2896650703680248</v>
       </c>
       <c r="D14">
-        <v>0.2518047907501916</v>
+        <v>0.2518047917296194</v>
       </c>
       <c r="E14">
-        <v>0.4514923485464675</v>
+        <v>0.4514923492569887</v>
       </c>
       <c r="F14">
-        <v>0.2328380501890041</v>
+        <v>0.232838051147319</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3167,19 +3167,19 @@
         <v>2024</v>
       </c>
       <c r="B15">
-        <v>0.3336982303562527</v>
+        <v>0.3336982315067402</v>
       </c>
       <c r="C15">
-        <v>0.5386659378680612</v>
+        <v>0.5386659387194874</v>
       </c>
       <c r="D15">
-        <v>0.4455564528666864</v>
+        <v>0.4455564538026689</v>
       </c>
       <c r="E15">
-        <v>0.9293522628533855</v>
+        <v>0.9293522631837802</v>
       </c>
       <c r="F15">
-        <v>0.403863369814531</v>
+        <v>0.4038633707482018</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3187,19 +3187,19 @@
         <v>2025</v>
       </c>
       <c r="B16">
-        <v>0.5214550409716485</v>
+        <v>0.5214550420845162</v>
       </c>
       <c r="C16">
-        <v>0.9791002768722074</v>
+        <v>0.9791002774281915</v>
       </c>
       <c r="D16">
-        <v>0.7714934008158958</v>
+        <v>0.7714934015623758</v>
       </c>
       <c r="E16">
-        <v>1.823916901928469</v>
+        <v>1.823916901511496</v>
       </c>
       <c r="F16">
-        <v>0.6872982507816439</v>
+        <v>0.6872982515669008</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3207,19 +3207,19 @@
         <v>2026</v>
       </c>
       <c r="B17">
-        <v>0.8043134554807252</v>
+        <v>0.8043134564479778</v>
       </c>
       <c r="C17">
-        <v>1.699994288989345</v>
+        <v>1.699994289077267</v>
       </c>
       <c r="D17">
-        <v>1.281585417850494</v>
+        <v>1.281585418277838</v>
       </c>
       <c r="E17">
-        <v>3.337011945587479</v>
+        <v>3.337011944111096</v>
       </c>
       <c r="F17">
-        <v>1.125247154131424</v>
+        <v>1.125247154661432</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3227,19 +3227,19 @@
         <v>2027</v>
       </c>
       <c r="B18">
-        <v>1.223805655308896</v>
+        <v>1.22380565603052</v>
       </c>
       <c r="C18">
-        <v>2.775502364461297</v>
+        <v>2.775502364038225</v>
       </c>
       <c r="D18">
-        <v>2.012536577429842</v>
+        <v>2.012536577498589</v>
       </c>
       <c r="E18">
-        <v>5.62447268438866</v>
+        <v>5.624472681845531</v>
       </c>
       <c r="F18">
-        <v>1.742919887402808</v>
+        <v>1.742919887653009</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3247,19 +3247,19 @@
         <v>2028</v>
       </c>
       <c r="B19">
-        <v>1.8347484617175</v>
+        <v>1.834748462121342</v>
       </c>
       <c r="C19">
-        <v>4.232870599883254</v>
+        <v>4.232870599143004</v>
       </c>
       <c r="D19">
-        <v>2.967977172449283</v>
+        <v>2.967977172278082</v>
       </c>
       <c r="E19">
-        <v>8.70621792466131</v>
+        <v>8.706217921606617</v>
       </c>
       <c r="F19">
-        <v>2.528793272724706</v>
+        <v>2.528793272815936</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3267,19 +3267,19 @@
         <v>2029</v>
       </c>
       <c r="B20">
-        <v>2.706137362035793</v>
+        <v>2.706137362094124</v>
       </c>
       <c r="C20">
-        <v>6.043642773180089</v>
+        <v>6.04364277257384</v>
       </c>
       <c r="D20">
-        <v>4.121517148912492</v>
+        <v>4.121517148786515</v>
       </c>
       <c r="E20">
-        <v>12.42531069254323</v>
+        <v>12.42531069016371</v>
       </c>
       <c r="F20">
-        <v>3.475513932027925</v>
+        <v>3.475513932235732</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3287,19 +3287,19 @@
         <v>2030</v>
       </c>
       <c r="B21">
-        <v>3.919965033173844</v>
+        <v>3.919965032915314</v>
       </c>
       <c r="C21">
-        <v>8.157895167909345</v>
+        <v>8.15789516801828</v>
       </c>
       <c r="D21">
-        <v>5.487469642182429</v>
+        <v>5.48746964254787</v>
       </c>
       <c r="E21">
-        <v>16.50602560322743</v>
+        <v>16.50602560306838</v>
       </c>
       <c r="F21">
-        <v>4.657918457187413</v>
+        <v>4.657918457595409</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3307,19 +3307,19 @@
         <v>2031</v>
       </c>
       <c r="B22">
-        <v>5.567414416908105</v>
+        <v>5.567414416425306</v>
       </c>
       <c r="C22">
-        <v>10.56645307742118</v>
+        <v>10.56645307871518</v>
       </c>
       <c r="D22">
-        <v>7.194951916824335</v>
+        <v>7.194951917778042</v>
       </c>
       <c r="E22">
-        <v>20.6856716549633</v>
+        <v>20.68567165837188</v>
       </c>
       <c r="F22">
-        <v>6.169517671849579</v>
+        <v>6.169517672510859</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3327,19 +3327,19 @@
         <v>2032</v>
       </c>
       <c r="B23">
-        <v>7.742579794517445</v>
+        <v>7.742579793969218</v>
       </c>
       <c r="C23">
-        <v>13.3473574401781</v>
+        <v>13.34735744278987</v>
       </c>
       <c r="D23">
-        <v>9.391961350620583</v>
+        <v>9.391961352085936</v>
       </c>
       <c r="E23">
-        <v>24.83599537259721</v>
+        <v>24.83599538015363</v>
       </c>
       <c r="F23">
-        <v>8.121156522385258</v>
+        <v>8.121156523330692</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3347,19 +3347,19 @@
         <v>2033</v>
       </c>
       <c r="B24">
-        <v>10.53445490911846</v>
+        <v>10.53445490872406</v>
       </c>
       <c r="C24">
-        <v>16.66448327696141</v>
+        <v>16.6644832806072</v>
       </c>
       <c r="D24">
-        <v>12.2402065769556</v>
+        <v>12.24020657876062</v>
       </c>
       <c r="E24">
-        <v>29.01406361058084</v>
+        <v>29.01406362180383</v>
       </c>
       <c r="F24">
-        <v>10.64038822067636</v>
+        <v>10.64038822186986</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3367,19 +3367,19 @@
         <v>2034</v>
       </c>
       <c r="B25">
-        <v>14.01825004568209</v>
+        <v>14.01825004570292</v>
       </c>
       <c r="C25">
-        <v>20.72365029700595</v>
+        <v>20.72365030108907</v>
       </c>
       <c r="D25">
-        <v>15.89571425101157</v>
+        <v>15.89571425291838</v>
       </c>
       <c r="E25">
-        <v>33.44618372069482</v>
+        <v>33.44618373412837</v>
       </c>
       <c r="F25">
-        <v>13.86275262573012</v>
+        <v>13.86275262707854</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3387,19 +3387,19 @@
         <v>2035</v>
       </c>
       <c r="B26">
-        <v>18.2473475798315</v>
+        <v>18.24734758053705</v>
       </c>
       <c r="C26">
-        <v>25.71361321301202</v>
+        <v>25.71361321684087</v>
       </c>
       <c r="D26">
-        <v>20.48145832107469</v>
+        <v>20.48145832284932</v>
       </c>
       <c r="E26">
-        <v>38.47210254900881</v>
+        <v>38.47210256260376</v>
       </c>
       <c r="F26">
-        <v>17.91743569944381</v>
+        <v>17.91743570078802</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3407,19 +3407,19 @@
         <v>2036</v>
       </c>
       <c r="B27">
-        <v>23.24726386400471</v>
+        <v>23.24726386562212</v>
       </c>
       <c r="C27">
-        <v>31.75456334587987</v>
+        <v>31.75456334889235</v>
       </c>
       <c r="D27">
-        <v>26.06502798465003</v>
+        <v>26.06502798613697</v>
       </c>
       <c r="E27">
-        <v>44.46238033828278</v>
+        <v>44.46238034990596</v>
       </c>
       <c r="F27">
-        <v>22.90309000258733</v>
+        <v>22.90309000376475</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3427,19 +3427,19 @@
         <v>2037</v>
       </c>
       <c r="B28">
-        <v>29.01261176958204</v>
+        <v>29.0126117722344</v>
       </c>
       <c r="C28">
-        <v>38.86412967540483</v>
+        <v>38.864129677316</v>
       </c>
       <c r="D28">
-        <v>32.63597377936185</v>
+        <v>32.6359737805341</v>
       </c>
       <c r="E28">
-        <v>51.71821097092904</v>
+        <v>51.71821097884627</v>
       </c>
       <c r="F28">
-        <v>28.86159563025346</v>
+        <v>28.86159563114361</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3447,19 +3447,19 @@
         <v>2038</v>
       </c>
       <c r="B29">
-        <v>35.50713082352723</v>
+        <v>35.50713082717284</v>
       </c>
       <c r="C29">
-        <v>46.94412437852603</v>
+        <v>46.94412437936634</v>
       </c>
       <c r="D29">
-        <v>40.10162999001214</v>
+        <v>40.10162999095573</v>
       </c>
       <c r="E29">
-        <v>60.37834194907803</v>
+        <v>60.37834195230003</v>
       </c>
       <c r="F29">
-        <v>35.76114540179062</v>
+        <v>35.76114540236402</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -3467,19 +3467,19 @@
         <v>2039</v>
       </c>
       <c r="B30">
-        <v>42.66569261570089</v>
+        <v>42.6656926200918</v>
       </c>
       <c r="C30">
-        <v>55.78863069918127</v>
+        <v>55.78863069923621</v>
       </c>
       <c r="D30">
-        <v>48.29296990563842</v>
+        <v>48.29296990650317</v>
       </c>
       <c r="E30">
-        <v>70.36446557318607</v>
+        <v>70.36446557161331</v>
       </c>
       <c r="F30">
-        <v>43.49135028498041</v>
+        <v>43.49135028526342</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3487,19 +3487,19 @@
         <v>2040</v>
       </c>
       <c r="B31">
-        <v>50.39633486731263</v>
+        <v>50.39633487199249</v>
       </c>
       <c r="C31">
-        <v>65.11084364619632</v>
+        <v>65.11084364588473</v>
       </c>
       <c r="D31">
-        <v>56.97896876172469</v>
+        <v>56.97896876267255</v>
       </c>
       <c r="E31">
-        <v>81.38149785076801</v>
+        <v>81.38149784512586</v>
       </c>
       <c r="F31">
-        <v>51.86665467016723</v>
+        <v>51.86665467023236</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3507,19 +3507,19 @@
         <v>2041</v>
       </c>
       <c r="B32">
-        <v>58.58049334324549</v>
+        <v>58.58049334760061</v>
       </c>
       <c r="C32">
-        <v>74.58229658671473</v>
+        <v>74.58229658645195</v>
       </c>
       <c r="D32">
-        <v>65.89143479527797</v>
+        <v>65.89143479641891</v>
       </c>
       <c r="E32">
-        <v>92.96609390475422</v>
+        <v>92.96609389636566</v>
       </c>
       <c r="F32">
-        <v>60.64312888763613</v>
+        <v>60.64312888757777</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3527,19 +3527,19 @@
         <v>2042</v>
       </c>
       <c r="B33">
-        <v>67.07089422914301</v>
+        <v>67.07089423250693</v>
       </c>
       <c r="C33">
-        <v>83.87592219159482</v>
+        <v>83.87592219168208</v>
       </c>
       <c r="D33">
-        <v>74.75232369246058</v>
+        <v>74.75232369382167</v>
       </c>
       <c r="E33">
-        <v>104.5630040049258</v>
+        <v>104.5630039954054</v>
       </c>
       <c r="F33">
-        <v>69.53662532231311</v>
+        <v>69.53662532224176</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3547,19 +3547,19 @@
         <v>2043</v>
       </c>
       <c r="B34">
-        <v>75.68874345744879</v>
+        <v>75.68874345924212</v>
       </c>
       <c r="C34">
-        <v>92.70461742912173</v>
+        <v>92.70461742968665</v>
       </c>
       <c r="D34">
-        <v>83.303893823211</v>
+        <v>83.30389382472757</v>
       </c>
       <c r="E34">
-        <v>115.6084195769151</v>
+        <v>115.6084195678682</v>
       </c>
       <c r="F34">
-        <v>78.24883781584876</v>
+        <v>78.24883781588548</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3567,19 +3567,19 @@
         <v>2044</v>
       </c>
       <c r="B35">
-        <v>84.22385056457256</v>
+        <v>84.22385056444352</v>
       </c>
       <c r="C35">
-        <v>100.849008497032</v>
+        <v>100.849008498026</v>
       </c>
       <c r="D35">
-        <v>91.33327549113309</v>
+        <v>91.33327549265931</v>
       </c>
       <c r="E35">
-        <v>125.605565051027</v>
+        <v>125.6055650438112</v>
       </c>
       <c r="F35">
-        <v>86.49811113220727</v>
+        <v>86.49811113246935</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3587,19 +3587,19 @@
         <v>2045</v>
       </c>
       <c r="B36">
-        <v>92.44190277822254</v>
+        <v>92.44190277614734</v>
       </c>
       <c r="C36">
-        <v>108.1710151389035</v>
+        <v>108.1710151401443</v>
       </c>
       <c r="D36">
-        <v>98.68726746750093</v>
+        <v>98.68726746885235</v>
       </c>
       <c r="E36">
-        <v>134.1834133761136</v>
+        <v>134.1834133716853</v>
       </c>
       <c r="F36">
-        <v>94.05012632920537</v>
+        <v>94.05012632978764</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3607,19 +3607,19 @@
         <v>2046</v>
       </c>
       <c r="B37">
-        <v>100.1014478619715</v>
+        <v>100.1014478582808</v>
       </c>
       <c r="C37">
-        <v>114.6129793903355</v>
+        <v>114.6129793915751</v>
       </c>
       <c r="D37">
-        <v>105.2768760976371</v>
+        <v>105.2768760986314</v>
       </c>
       <c r="E37">
-        <v>141.1327183845186</v>
+        <v>141.1327183833626</v>
       </c>
       <c r="F37">
-        <v>100.7403404835654</v>
+        <v>100.74034048452</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3627,19 +3627,19 @@
         <v>2047</v>
       </c>
       <c r="B38">
-        <v>106.9796155115961</v>
+        <v>106.9796155069151</v>
       </c>
       <c r="C38">
-        <v>120.1850103389176</v>
+        <v>120.1850103399127</v>
       </c>
       <c r="D38">
-        <v>111.0716549500159</v>
+        <v>111.0716549505161</v>
       </c>
       <c r="E38">
-        <v>146.4163091965139</v>
+        <v>146.4163091986451</v>
       </c>
       <c r="F38">
-        <v>106.4868384080489</v>
+        <v>106.4868384093697</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -3647,19 +3647,19 @@
         <v>2048</v>
       </c>
       <c r="B39">
-        <v>112.9016652874762</v>
+        <v>112.9016652825919</v>
       </c>
       <c r="C39">
-        <v>124.9452423750547</v>
+        <v>124.9452423756247</v>
       </c>
       <c r="D39">
-        <v>116.0869986308877</v>
+        <v>116.0869986308346</v>
       </c>
       <c r="E39">
-        <v>150.1543637152629</v>
+        <v>150.1543637202831</v>
       </c>
       <c r="F39">
-        <v>111.2897153400317</v>
+        <v>111.2897153416466</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3667,19 +3667,19 @@
         <v>2049</v>
       </c>
       <c r="B40">
-        <v>117.7669663997275</v>
+        <v>117.7669663954195</v>
       </c>
       <c r="C40">
-        <v>128.9784272795504</v>
+        <v>128.9784272796098</v>
       </c>
       <c r="D40">
-        <v>120.368991200558</v>
+        <v>120.3689911999818</v>
       </c>
       <c r="E40">
-        <v>152.5897298530816</v>
+        <v>152.5897298602756</v>
       </c>
       <c r="F40">
-        <v>115.218842951363</v>
+        <v>115.2188429531423</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -3687,19 +3687,19 @@
         <v>2050</v>
       </c>
       <c r="B41">
-        <v>121.5642085708811</v>
+        <v>121.5642085677618</v>
       </c>
       <c r="C41">
-        <v>132.3775594827742</v>
+        <v>132.3775594823399</v>
       </c>
       <c r="D41">
-        <v>123.9806145657172</v>
+        <v>123.9806145647298</v>
       </c>
       <c r="E41">
-        <v>154.0416006414277</v>
+        <v>154.0416006498818</v>
       </c>
       <c r="F41">
-        <v>118.3937840686607</v>
+        <v>118.3937840704334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>